<commit_message>
Compute energy and memory usage for each model
</commit_message>
<xml_diff>
--- a/2-4 GHz Analysis/tables/models_metrics_in_test_set_Geral.xlsx
+++ b/2-4 GHz Analysis/tables/models_metrics_in_test_set_Geral.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,16 @@
           <t>R2</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Execution Time (ms)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Memory Usage (B)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -470,6 +480,12 @@
       <c r="D2" t="n">
         <v>0.6063990250024073</v>
       </c>
+      <c r="E2" t="n">
+        <v>6.878599990159273</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -486,6 +502,12 @@
       <c r="D3" t="n">
         <v>0.8867600587631547</v>
       </c>
+      <c r="E3" t="n">
+        <v>7.01979998848401</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -502,6 +524,12 @@
       <c r="D4" t="n">
         <v>0.9027505685981926</v>
       </c>
+      <c r="E4" t="n">
+        <v>45.48119998071343</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -517,6 +545,12 @@
       </c>
       <c r="D5" t="n">
         <v>0.8563441713648984</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3.086799988523126</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>